<commit_message>
commiting changes for Jenkins
</commit_message>
<xml_diff>
--- a/InputFiles/CCDI/TC02_CCDI_phs000720_Filetype-dicom_Tumorclassf-Metastatic.xlsx
+++ b/InputFiles/CCDI/TC02_CCDI_phs000720_Filetype-dicom_Tumorclassf-Metastatic.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tatekaraa\Automation\03-31-25\Commons_Automation\InputFiles\CCDI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tatekaraa\Automation\05-01-25\Commons_Automation\InputFiles\CCDI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B11FBC5-0D4A-4898-AA6E-2645ACD7AC68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AC5455D-2F52-4351-BFC5-22091D298DFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -196,10 +196,7 @@
     std.dbgap_accession = 'phs000720' and smp.tumor_classification = 'Metastatic' and path.file_type ='dicom';</t>
   </si>
   <si>
-    <t>with file_data as (
-select file_name, data_category,file_type, file_size,file_access,  file_description,"sample.id" from df_sequencing_file
-union
-select file_name, data_category,file_type, file_size,file_access,  file_description,"sample.id" from df_pathology_file)
+    <t>with file_data as (select file_name, data_category,file_type, file_size,file_access,  file_description,"sample.id" from df_pathology_file)
 SELECT DISTINCT
     fd.file_name AS "File Name",
     fd.data_category AS "Data Category",
@@ -207,13 +204,13 @@
     fd.file_type AS "File Type",
     CASE     
         WHEN fd.file_size &gt;= 1024 * 1024 * 1024 THEN 
-            ROUND(fd.file_size / (1024.0 * 1024.0 * 1024.0), 2) || ' GB' 
+            RTRIM(RTRIM(printf('%.2f', fd.file_size / (1024.0 * 1024.0 * 1024.0)), '0'), '.') || ' GB'
         WHEN fd.file_size &gt;= 1024 * 1024 THEN 
-            ROUND(fd.file_size / (1024.0 * 1024.0), 2) || ' MB' 
+            RTRIM(RTRIM(printf('%.2f', fd.file_size / (1024.0 * 1024.0)), '0'), '.') || ' MB'
         WHEN fd.file_size &gt;= 1024 THEN 
-            ROUND(fd.file_size / 1024.0, 2) || ' KB' 
+            RTRIM(RTRIM(printf('%.2f', fd.file_size / 1024.0), '0'), '.') || ' KB'
         ELSE 
-            ROUND(fd.file_size, 2) || ' Bytes' 
+            RTRIM(RTRIM(printf('%.2f', fd.file_size), '0'), '.') || ' Bytes'
     END AS "File Size",
     fd.file_access AS "File Access",
     std.dbgap_accession AS "Study ID",
@@ -228,8 +225,10 @@
 JOIN 
     file_data fd ON smp.id = fd."sample.id"
 WHERE 
-    std.dbgap_accession = 'phs000720' and fd.file_type ='dicom' and smp.tumor_classification = 'Metastatic'
-LIMIT 100;</t>
+    std.dbgap_accession = 'phs000720' 
+    AND fd.file_type = 'dicom' 
+    AND smp.tumor_classification = 'Metastatic'
+Order by fd.file_name asc LIMIT 100;</t>
   </si>
 </sst>
 </file>
@@ -632,18 +631,18 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="75.85546875" customWidth="1"/>
-    <col min="4" max="4" width="70.140625" customWidth="1"/>
-    <col min="5" max="5" width="63.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="75.81640625" customWidth="1"/>
+    <col min="4" max="4" width="70.1796875" customWidth="1"/>
+    <col min="5" max="5" width="63.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -660,7 +659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -677,7 +676,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -686,7 +685,7 @@
       </c>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -695,7 +694,7 @@
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -704,11 +703,11 @@
       </c>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C7" s="1"/>
     </row>
   </sheetData>

</xml_diff>